<commit_message>
GUI to search for symbols from a range of free datasources including trading view. Operable from jupyter nb & returns dict of chosen series metadata. It s on....
</commit_message>
<xml_diff>
--- a/MacroBackend/BEA_Data/Datasets/BEAAPI_Info.xlsx
+++ b/MacroBackend/BEA_Data/Datasets/BEAAPI_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/Bootleg_Macro/MacroBackend/BEA_Data/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B2F47F-DADC-2B4D-8ABF-0F1B62C06CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19B218F-2E66-2742-9287-AD7FA731E821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSetList" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,25 @@
     <sheet name="Regional_params" sheetId="14" r:id="rId14"/>
     <sheet name="UnderlyingGDPbyIndustry_params" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="1104">
   <si>
     <t>DatasetName</t>
   </si>
@@ -3714,6 +3727,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -4050,7 +4067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4588,8 +4607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8047,845 +8066,623 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="142" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>652</v>
       </c>
       <c r="B2" t="s">
-        <v>652</v>
-      </c>
-      <c r="C2" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>654</v>
       </c>
       <c r="B3" t="s">
-        <v>654</v>
-      </c>
-      <c r="C3" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>656</v>
       </c>
       <c r="B4" t="s">
-        <v>656</v>
-      </c>
-      <c r="C4" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>658</v>
       </c>
       <c r="B5" t="s">
-        <v>658</v>
-      </c>
-      <c r="C5" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>660</v>
       </c>
       <c r="B6" t="s">
-        <v>660</v>
-      </c>
-      <c r="C6" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>662</v>
       </c>
       <c r="B7" t="s">
-        <v>662</v>
-      </c>
-      <c r="C7" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>664</v>
       </c>
       <c r="B8" t="s">
-        <v>664</v>
-      </c>
-      <c r="C8" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>666</v>
       </c>
       <c r="B9" t="s">
-        <v>666</v>
-      </c>
-      <c r="C9" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>668</v>
       </c>
       <c r="B10" t="s">
-        <v>668</v>
-      </c>
-      <c r="C10" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>670</v>
       </c>
       <c r="B11" t="s">
-        <v>670</v>
-      </c>
-      <c r="C11" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>672</v>
       </c>
       <c r="B12" t="s">
-        <v>672</v>
-      </c>
-      <c r="C12" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>674</v>
       </c>
       <c r="B13" t="s">
-        <v>674</v>
-      </c>
-      <c r="C13" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>676</v>
       </c>
       <c r="B14" t="s">
-        <v>676</v>
-      </c>
-      <c r="C14" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>678</v>
       </c>
       <c r="B15" t="s">
-        <v>678</v>
-      </c>
-      <c r="C15" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>680</v>
       </c>
       <c r="B16" t="s">
-        <v>680</v>
-      </c>
-      <c r="C16" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>682</v>
       </c>
       <c r="B17" t="s">
-        <v>682</v>
-      </c>
-      <c r="C17" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>684</v>
       </c>
       <c r="B18" t="s">
-        <v>684</v>
-      </c>
-      <c r="C18" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>686</v>
       </c>
       <c r="B19" t="s">
-        <v>686</v>
-      </c>
-      <c r="C19" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>688</v>
       </c>
       <c r="B20" t="s">
-        <v>688</v>
-      </c>
-      <c r="C20" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>690</v>
       </c>
       <c r="B21" t="s">
-        <v>690</v>
-      </c>
-      <c r="C21" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>692</v>
       </c>
       <c r="B22" t="s">
-        <v>692</v>
-      </c>
-      <c r="C22" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>694</v>
       </c>
       <c r="B23" t="s">
-        <v>694</v>
-      </c>
-      <c r="C23" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>696</v>
       </c>
       <c r="B24" t="s">
-        <v>696</v>
-      </c>
-      <c r="C24" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>698</v>
       </c>
       <c r="B25" t="s">
-        <v>698</v>
-      </c>
-      <c r="C25" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>700</v>
       </c>
       <c r="B26" t="s">
-        <v>700</v>
-      </c>
-      <c r="C26" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>702</v>
       </c>
       <c r="B27" t="s">
-        <v>702</v>
-      </c>
-      <c r="C27" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>704</v>
       </c>
       <c r="B28" t="s">
-        <v>704</v>
-      </c>
-      <c r="C28" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>706</v>
       </c>
       <c r="B29" t="s">
-        <v>706</v>
-      </c>
-      <c r="C29" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>708</v>
       </c>
       <c r="B30" t="s">
-        <v>708</v>
-      </c>
-      <c r="C30" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>710</v>
       </c>
       <c r="B31" t="s">
-        <v>710</v>
-      </c>
-      <c r="C31" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>712</v>
       </c>
       <c r="B32" t="s">
-        <v>712</v>
-      </c>
-      <c r="C32" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>714</v>
       </c>
       <c r="B33" t="s">
-        <v>714</v>
-      </c>
-      <c r="C33" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>716</v>
       </c>
       <c r="B34" t="s">
-        <v>716</v>
-      </c>
-      <c r="C34" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>718</v>
       </c>
       <c r="B35" t="s">
-        <v>718</v>
-      </c>
-      <c r="C35" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>720</v>
       </c>
       <c r="B36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C36" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>722</v>
       </c>
       <c r="B37" t="s">
-        <v>722</v>
-      </c>
-      <c r="C37" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>724</v>
       </c>
       <c r="B38" t="s">
-        <v>724</v>
-      </c>
-      <c r="C38" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>726</v>
       </c>
       <c r="B39" t="s">
-        <v>726</v>
-      </c>
-      <c r="C39" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>728</v>
       </c>
       <c r="B40" t="s">
-        <v>728</v>
-      </c>
-      <c r="C40" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>730</v>
       </c>
       <c r="B41" t="s">
-        <v>730</v>
-      </c>
-      <c r="C41" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>732</v>
       </c>
       <c r="B42" t="s">
-        <v>732</v>
-      </c>
-      <c r="C42" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>734</v>
       </c>
       <c r="B43" t="s">
-        <v>734</v>
-      </c>
-      <c r="C43" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>736</v>
       </c>
       <c r="B44" t="s">
-        <v>736</v>
-      </c>
-      <c r="C44" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>738</v>
       </c>
       <c r="B45" t="s">
-        <v>738</v>
-      </c>
-      <c r="C45" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>740</v>
       </c>
       <c r="B46" t="s">
-        <v>740</v>
-      </c>
-      <c r="C46" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>742</v>
       </c>
       <c r="B47" t="s">
-        <v>742</v>
-      </c>
-      <c r="C47" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>744</v>
       </c>
       <c r="B48" t="s">
-        <v>744</v>
-      </c>
-      <c r="C48" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>746</v>
       </c>
       <c r="B49" t="s">
-        <v>746</v>
-      </c>
-      <c r="C49" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>748</v>
       </c>
       <c r="B50" t="s">
-        <v>748</v>
-      </c>
-      <c r="C50" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>750</v>
       </c>
       <c r="B51" t="s">
-        <v>750</v>
-      </c>
-      <c r="C51" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>752</v>
       </c>
       <c r="B52" t="s">
-        <v>752</v>
-      </c>
-      <c r="C52" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>754</v>
       </c>
       <c r="B53" t="s">
-        <v>754</v>
-      </c>
-      <c r="C53" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>756</v>
       </c>
       <c r="B54" t="s">
-        <v>756</v>
-      </c>
-      <c r="C54" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>758</v>
       </c>
       <c r="B55" t="s">
-        <v>758</v>
-      </c>
-      <c r="C55" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>760</v>
       </c>
       <c r="B56" t="s">
-        <v>760</v>
-      </c>
-      <c r="C56" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>762</v>
       </c>
       <c r="B57" t="s">
-        <v>762</v>
-      </c>
-      <c r="C57" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>764</v>
       </c>
       <c r="B58" t="s">
-        <v>764</v>
-      </c>
-      <c r="C58" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>766</v>
       </c>
       <c r="B59" t="s">
-        <v>766</v>
-      </c>
-      <c r="C59" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>768</v>
       </c>
       <c r="B60" t="s">
-        <v>768</v>
-      </c>
-      <c r="C60" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>770</v>
       </c>
       <c r="B61" t="s">
-        <v>770</v>
-      </c>
-      <c r="C61" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>772</v>
       </c>
       <c r="B62" t="s">
-        <v>772</v>
-      </c>
-      <c r="C62" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>774</v>
       </c>
       <c r="B63" t="s">
-        <v>774</v>
-      </c>
-      <c r="C63" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>776</v>
       </c>
       <c r="B64" t="s">
-        <v>776</v>
-      </c>
-      <c r="C64" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>778</v>
       </c>
       <c r="B65" t="s">
-        <v>778</v>
-      </c>
-      <c r="C65" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>780</v>
       </c>
       <c r="B66" t="s">
-        <v>780</v>
-      </c>
-      <c r="C66" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>782</v>
       </c>
       <c r="B67" t="s">
-        <v>782</v>
-      </c>
-      <c r="C67" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>784</v>
       </c>
       <c r="B68" t="s">
-        <v>784</v>
-      </c>
-      <c r="C68" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>786</v>
       </c>
       <c r="B69" t="s">
-        <v>786</v>
-      </c>
-      <c r="C69" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>788</v>
       </c>
       <c r="B70" t="s">
-        <v>788</v>
-      </c>
-      <c r="C70" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>790</v>
       </c>
       <c r="B71" t="s">
-        <v>790</v>
-      </c>
-      <c r="C71" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>792</v>
       </c>
       <c r="B72" t="s">
-        <v>792</v>
-      </c>
-      <c r="C72" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>794</v>
       </c>
       <c r="B73" t="s">
-        <v>794</v>
-      </c>
-      <c r="C73" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>796</v>
       </c>
       <c r="B74" t="s">
-        <v>796</v>
-      </c>
-      <c r="C74" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>798</v>
       </c>
       <c r="B75" t="s">
-        <v>798</v>
-      </c>
-      <c r="C75" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>800</v>
       </c>
       <c r="B76" t="s">
-        <v>800</v>
-      </c>
-      <c r="C76" t="s">
         <v>801</v>
       </c>
     </row>
@@ -8896,1219 +8693,895 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="116.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>802</v>
       </c>
       <c r="B2" t="s">
-        <v>802</v>
-      </c>
-      <c r="C2" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>804</v>
       </c>
       <c r="B3" t="s">
-        <v>804</v>
-      </c>
-      <c r="C3" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>806</v>
       </c>
       <c r="B4" t="s">
-        <v>806</v>
-      </c>
-      <c r="C4" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>808</v>
       </c>
       <c r="B5" t="s">
-        <v>808</v>
-      </c>
-      <c r="C5" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>810</v>
       </c>
       <c r="B6" t="s">
-        <v>810</v>
-      </c>
-      <c r="C6" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>812</v>
       </c>
       <c r="B7" t="s">
-        <v>812</v>
-      </c>
-      <c r="C7" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>814</v>
       </c>
       <c r="B8" t="s">
-        <v>814</v>
-      </c>
-      <c r="C8" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>816</v>
       </c>
       <c r="B9" t="s">
-        <v>816</v>
-      </c>
-      <c r="C9" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>818</v>
       </c>
       <c r="B10" t="s">
-        <v>818</v>
-      </c>
-      <c r="C10" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>820</v>
       </c>
       <c r="B11" t="s">
-        <v>820</v>
-      </c>
-      <c r="C11" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>822</v>
       </c>
       <c r="B12" t="s">
-        <v>822</v>
-      </c>
-      <c r="C12" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>824</v>
       </c>
       <c r="B13" t="s">
-        <v>824</v>
-      </c>
-      <c r="C13" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>826</v>
       </c>
       <c r="B14" t="s">
-        <v>826</v>
-      </c>
-      <c r="C14" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>828</v>
       </c>
       <c r="B15" t="s">
-        <v>828</v>
-      </c>
-      <c r="C15" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>830</v>
       </c>
       <c r="B16" t="s">
-        <v>830</v>
-      </c>
-      <c r="C16" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>832</v>
       </c>
       <c r="B17" t="s">
-        <v>832</v>
-      </c>
-      <c r="C17" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>834</v>
       </c>
       <c r="B18" t="s">
-        <v>834</v>
-      </c>
-      <c r="C18" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>836</v>
       </c>
       <c r="B19" t="s">
-        <v>836</v>
-      </c>
-      <c r="C19" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>838</v>
       </c>
       <c r="B20" t="s">
-        <v>838</v>
-      </c>
-      <c r="C20" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>840</v>
       </c>
       <c r="B21" t="s">
-        <v>840</v>
-      </c>
-      <c r="C21" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>842</v>
       </c>
       <c r="B22" t="s">
-        <v>842</v>
-      </c>
-      <c r="C22" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>844</v>
       </c>
       <c r="B23" t="s">
-        <v>844</v>
-      </c>
-      <c r="C23" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>846</v>
       </c>
       <c r="B24" t="s">
-        <v>846</v>
-      </c>
-      <c r="C24" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>848</v>
       </c>
       <c r="B25" t="s">
-        <v>848</v>
-      </c>
-      <c r="C25" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>850</v>
       </c>
       <c r="B26" t="s">
-        <v>850</v>
-      </c>
-      <c r="C26" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>852</v>
       </c>
       <c r="B27" t="s">
-        <v>852</v>
-      </c>
-      <c r="C27" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>854</v>
       </c>
       <c r="B28" t="s">
-        <v>854</v>
-      </c>
-      <c r="C28" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>856</v>
       </c>
       <c r="B29" t="s">
-        <v>856</v>
-      </c>
-      <c r="C29" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>858</v>
       </c>
       <c r="B30" t="s">
-        <v>858</v>
-      </c>
-      <c r="C30" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>860</v>
       </c>
       <c r="B31" t="s">
-        <v>860</v>
-      </c>
-      <c r="C31" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>862</v>
       </c>
       <c r="B32" t="s">
-        <v>862</v>
-      </c>
-      <c r="C32" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>864</v>
       </c>
       <c r="B33" t="s">
-        <v>864</v>
-      </c>
-      <c r="C33" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>866</v>
       </c>
       <c r="B34" t="s">
-        <v>866</v>
-      </c>
-      <c r="C34" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>868</v>
       </c>
       <c r="B35" t="s">
-        <v>868</v>
-      </c>
-      <c r="C35" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>870</v>
       </c>
       <c r="B36" t="s">
-        <v>870</v>
-      </c>
-      <c r="C36" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>872</v>
       </c>
       <c r="B37" t="s">
-        <v>872</v>
-      </c>
-      <c r="C37" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>874</v>
       </c>
       <c r="B38" t="s">
-        <v>874</v>
-      </c>
-      <c r="C38" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>876</v>
       </c>
       <c r="B39" t="s">
-        <v>876</v>
-      </c>
-      <c r="C39" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>878</v>
       </c>
       <c r="B40" t="s">
-        <v>878</v>
-      </c>
-      <c r="C40" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>880</v>
       </c>
       <c r="B41" t="s">
-        <v>880</v>
-      </c>
-      <c r="C41" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>882</v>
       </c>
       <c r="B42" t="s">
-        <v>882</v>
-      </c>
-      <c r="C42" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>884</v>
       </c>
       <c r="B43" t="s">
-        <v>884</v>
-      </c>
-      <c r="C43" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>886</v>
       </c>
       <c r="B44" t="s">
-        <v>886</v>
-      </c>
-      <c r="C44" t="s">
         <v>887</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>888</v>
       </c>
       <c r="B45" t="s">
-        <v>888</v>
-      </c>
-      <c r="C45" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>890</v>
       </c>
       <c r="B46" t="s">
-        <v>890</v>
-      </c>
-      <c r="C46" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>892</v>
       </c>
       <c r="B47" t="s">
-        <v>892</v>
-      </c>
-      <c r="C47" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>894</v>
       </c>
       <c r="B48" t="s">
-        <v>894</v>
-      </c>
-      <c r="C48" t="s">
         <v>895</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>896</v>
       </c>
       <c r="B49" t="s">
-        <v>896</v>
-      </c>
-      <c r="C49" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>898</v>
       </c>
       <c r="B50" t="s">
-        <v>898</v>
-      </c>
-      <c r="C50" t="s">
         <v>899</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>900</v>
       </c>
       <c r="B51" t="s">
-        <v>900</v>
-      </c>
-      <c r="C51" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>902</v>
       </c>
       <c r="B52" t="s">
-        <v>902</v>
-      </c>
-      <c r="C52" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>904</v>
       </c>
       <c r="B53" t="s">
-        <v>904</v>
-      </c>
-      <c r="C53" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>906</v>
       </c>
       <c r="B54" t="s">
-        <v>906</v>
-      </c>
-      <c r="C54" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>908</v>
       </c>
       <c r="B55" t="s">
-        <v>908</v>
-      </c>
-      <c r="C55" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>910</v>
       </c>
       <c r="B56" t="s">
-        <v>910</v>
-      </c>
-      <c r="C56" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>912</v>
       </c>
       <c r="B57" t="s">
-        <v>912</v>
-      </c>
-      <c r="C57" t="s">
         <v>913</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>914</v>
       </c>
       <c r="B58" t="s">
-        <v>914</v>
-      </c>
-      <c r="C58" t="s">
         <v>915</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>916</v>
       </c>
       <c r="B59" t="s">
-        <v>916</v>
-      </c>
-      <c r="C59" t="s">
         <v>917</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>918</v>
       </c>
       <c r="B60" t="s">
-        <v>918</v>
-      </c>
-      <c r="C60" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>920</v>
       </c>
       <c r="B61" t="s">
-        <v>920</v>
-      </c>
-      <c r="C61" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>922</v>
       </c>
       <c r="B62" t="s">
-        <v>922</v>
-      </c>
-      <c r="C62" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>924</v>
       </c>
       <c r="B63" t="s">
-        <v>924</v>
-      </c>
-      <c r="C63" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>926</v>
       </c>
       <c r="B64" t="s">
-        <v>926</v>
-      </c>
-      <c r="C64" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>928</v>
       </c>
       <c r="B65" t="s">
-        <v>928</v>
-      </c>
-      <c r="C65" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>930</v>
       </c>
       <c r="B66" t="s">
-        <v>930</v>
-      </c>
-      <c r="C66" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>932</v>
       </c>
       <c r="B67" t="s">
-        <v>932</v>
-      </c>
-      <c r="C67" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>934</v>
       </c>
       <c r="B68" t="s">
-        <v>934</v>
-      </c>
-      <c r="C68" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>936</v>
       </c>
       <c r="B69" t="s">
-        <v>936</v>
-      </c>
-      <c r="C69" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>938</v>
       </c>
       <c r="B70" t="s">
-        <v>938</v>
-      </c>
-      <c r="C70" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>940</v>
       </c>
       <c r="B71" t="s">
-        <v>940</v>
-      </c>
-      <c r="C71" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>942</v>
       </c>
       <c r="B72" t="s">
-        <v>942</v>
-      </c>
-      <c r="C72" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>944</v>
       </c>
       <c r="B73" t="s">
-        <v>944</v>
-      </c>
-      <c r="C73" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>946</v>
       </c>
       <c r="B74" t="s">
-        <v>946</v>
-      </c>
-      <c r="C74" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>948</v>
       </c>
       <c r="B75" t="s">
-        <v>948</v>
-      </c>
-      <c r="C75" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>950</v>
       </c>
       <c r="B76" t="s">
-        <v>950</v>
-      </c>
-      <c r="C76" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>952</v>
       </c>
       <c r="B77" t="s">
-        <v>952</v>
-      </c>
-      <c r="C77" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>954</v>
       </c>
       <c r="B78" t="s">
-        <v>954</v>
-      </c>
-      <c r="C78" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>956</v>
       </c>
       <c r="B79" t="s">
-        <v>956</v>
-      </c>
-      <c r="C79" t="s">
         <v>957</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>958</v>
       </c>
       <c r="B80" t="s">
-        <v>958</v>
-      </c>
-      <c r="C80" t="s">
         <v>959</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>960</v>
       </c>
       <c r="B81" t="s">
-        <v>960</v>
-      </c>
-      <c r="C81" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>962</v>
       </c>
       <c r="B82" t="s">
-        <v>962</v>
-      </c>
-      <c r="C82" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>964</v>
       </c>
       <c r="B83" t="s">
-        <v>964</v>
-      </c>
-      <c r="C83" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>966</v>
       </c>
       <c r="B84" t="s">
-        <v>966</v>
-      </c>
-      <c r="C84" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>968</v>
       </c>
       <c r="B85" t="s">
-        <v>968</v>
-      </c>
-      <c r="C85" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>970</v>
       </c>
       <c r="B86" t="s">
-        <v>970</v>
-      </c>
-      <c r="C86" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>972</v>
       </c>
       <c r="B87" t="s">
-        <v>972</v>
-      </c>
-      <c r="C87" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>974</v>
       </c>
       <c r="B88" t="s">
-        <v>974</v>
-      </c>
-      <c r="C88" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>976</v>
       </c>
       <c r="B89" t="s">
-        <v>976</v>
-      </c>
-      <c r="C89" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>978</v>
       </c>
       <c r="B90" t="s">
-        <v>978</v>
-      </c>
-      <c r="C90" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>980</v>
       </c>
       <c r="B91" t="s">
-        <v>980</v>
-      </c>
-      <c r="C91" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>982</v>
       </c>
       <c r="B92" t="s">
-        <v>982</v>
-      </c>
-      <c r="C92" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>984</v>
       </c>
       <c r="B93" t="s">
-        <v>984</v>
-      </c>
-      <c r="C93" t="s">
         <v>985</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>986</v>
       </c>
       <c r="B94" t="s">
-        <v>986</v>
-      </c>
-      <c r="C94" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>988</v>
       </c>
       <c r="B95" t="s">
-        <v>988</v>
-      </c>
-      <c r="C95" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>990</v>
       </c>
       <c r="B96" t="s">
-        <v>990</v>
-      </c>
-      <c r="C96" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>992</v>
       </c>
       <c r="B97" t="s">
-        <v>992</v>
-      </c>
-      <c r="C97" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>994</v>
       </c>
       <c r="B98" t="s">
-        <v>994</v>
-      </c>
-      <c r="C98" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>996</v>
       </c>
       <c r="B99" t="s">
-        <v>996</v>
-      </c>
-      <c r="C99" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>998</v>
       </c>
       <c r="B100" t="s">
-        <v>998</v>
-      </c>
-      <c r="C100" t="s">
         <v>999</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>1000</v>
       </c>
       <c r="B101" t="s">
-        <v>1000</v>
-      </c>
-      <c r="C101" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>1002</v>
       </c>
       <c r="B102" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C102" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>1004</v>
       </c>
       <c r="B103" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C103" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>1006</v>
       </c>
       <c r="B104" t="s">
-        <v>1006</v>
-      </c>
-      <c r="C104" t="s">
         <v>1007</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>1008</v>
       </c>
       <c r="B105" t="s">
-        <v>1008</v>
-      </c>
-      <c r="C105" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>1010</v>
       </c>
       <c r="B106" t="s">
-        <v>1010</v>
-      </c>
-      <c r="C106" t="s">
         <v>1011</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>1012</v>
       </c>
       <c r="B107" t="s">
-        <v>1012</v>
-      </c>
-      <c r="C107" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>1014</v>
       </c>
       <c r="B108" t="s">
-        <v>1014</v>
-      </c>
-      <c r="C108" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>1016</v>
       </c>
       <c r="B109" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C109" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>1018</v>
       </c>
       <c r="B110" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C110" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -10124,6 +9597,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">

</xml_diff>